<commit_message>
I am sorry  :::((( Ручное слияние FilterObj --> master
</commit_message>
<xml_diff>
--- a/fias_loader/TESTS/Y_BUILD/05/_TEST_xxx_adr_area_type.xlsx
+++ b/fias_loader/TESTS/Y_BUILD/05/_TEST_xxx_adr_area_type.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1742,7 +1742,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1763,62 +1763,8 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="15">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1827,62 +1773,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFFCD4D1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFED1C24"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFBEE3D3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFCD4D1"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBEE3D3"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFED1C24"/>
-        <bgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -1904,7 +1808,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1912,23 +1816,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1952,50 +1841,33 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2004,30 +1876,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2035,26 +1890,26 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF00AAAD"/>
-      <rgbColor rgb="FFFCD4D1"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFBEE3D3"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066B3"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -2065,12 +1920,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFBEE3D3"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFCD4D1"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -2099,8 +1954,8 @@
   </sheetPr>
   <dimension ref="A1:I143"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C95" activeCellId="0" sqref="C95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C138" activeCellId="0" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4846,25 +4701,25 @@
       <c r="A95" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B95" s="4" t="n">
+      <c r="B95" s="2" t="n">
         <v>94</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C95" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="D95" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="E95" s="4" t="s">
+      <c r="E95" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="F95" s="4" t="s">
+      <c r="F95" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="G95" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H95" s="4" t="s">
+      <c r="G95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" s="2" t="s">
         <v>384</v>
       </c>
       <c r="I95" s="2" t="s">
@@ -6265,11 +6120,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CСтраница &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>